<commit_message>
orient all diff's the same way: diff REF ACTUAL
also modify "msl38/proposalsTest6_split/" test case to change spaces in made-up species names into dashes to comply with binomial naming rules.
</commit_message>
<xml_diff>
--- a/testData/msl38/proposalsTest6_split/2023.907D.N.v1.Correct_split.xlsx
+++ b/testData/msl38/proposalsTest6_split/2023.907D.N.v1.Correct_split.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curtish/Documents/ICTV/validate_proposals/testData/proposalsTest6_split/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curtish/Documents/ICTV/load_msl/testData/msl38/proposalsTest6_split/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26031554-4247-0945-A53E-BE92E8D13C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE337ED-116C-BA4B-90D1-92B8857B1CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="1600" windowWidth="29400" windowHeight="13260" activeTab="1" xr2:uid="{94A59F7B-7A42-3941-BED7-E7ACB004C4FA}"/>
+    <workbookView xWindow="520" yWindow="1600" windowWidth="29400" windowHeight="13260" activeTab="1" xr2:uid="{94A59F7B-7A42-3941-BED7-E7ACB004C4FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <definedName name="studySectionCodeList" comment="list of valid 1-letter codes for study sections, for input validation.">'Menu Items (Do not change)'!$F:$F</definedName>
     <definedName name="studySectionCodeLUT" comment="Define columns in [Menu Items] that map Study Section letters to full names">'Menu Items (Do not change)'!$F:$G</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1679,21 +1679,12 @@
     <t>exemplar 1</t>
   </si>
   <si>
-    <t>Hemiambidensovirus hemipteran split1</t>
-  </si>
-  <si>
-    <t>Hemiambidensovirus hemipteran split2</t>
-  </si>
-  <si>
     <t>exemplar split1</t>
   </si>
   <si>
     <t>exemplar split2</t>
   </si>
   <si>
-    <t>Hemiambidensovirus hemipteran split3 dup acc</t>
-  </si>
-  <si>
     <t>FJ040397</t>
   </si>
   <si>
@@ -1788,6 +1779,15 @@
   </si>
   <si>
     <t>split species into only new names, but keep accession</t>
+  </si>
+  <si>
+    <t>Hemiambidensovirus hemipteran-split1</t>
+  </si>
+  <si>
+    <t>Hemiambidensovirus hemipteran-split2</t>
+  </si>
+  <si>
+    <t>Hemiambidensovirus hemipteran-split3-dup-acc</t>
   </si>
 </sst>
 </file>
@@ -2285,7 +2285,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2367,6 +2367,34 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2409,50 +2437,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% - Accent3" xfId="1" builtinId="40"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-      </font>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2492,29 +2483,15 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF7030A0"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF7030A0"/>
+        <b val="0"/>
+        <i/>
       </font>
     </dxf>
     <dxf>
@@ -2543,9 +2520,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2583,7 +2560,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2689,7 +2666,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2831,7 +2808,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2861,7 +2838,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>ROW(B2)&gt;5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2875,7 +2852,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T9" sqref="T9"/>
+      <selection pane="bottomLeft" activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2908,7 +2885,7 @@
     <col min="27" max="27" width="16.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19" style="14" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="10" style="14" customWidth="1"/>
-    <col min="30" max="30" width="30.5" style="26" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="41.1640625" style="26" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10.33203125" style="4" customWidth="1"/>
     <col min="32" max="32" width="32.83203125" style="4" customWidth="1"/>
     <col min="33" max="33" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
@@ -2925,26 +2902,26 @@
       <c r="A1" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="90" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="63" t="str">
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="91" t="str">
         <f ca="1">IF(LEN(cellFilenameFormatErrors)=0,LEFT(cellBaseFilename,9),"Code is automatically derived from the filename: 'YEAR.###X.[STATUS.][v#.]DESCRIPTION.xlsx', X=SC code")</f>
         <v>2023.907D</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="53" t="str">
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="81" t="str">
         <f ca="1">IF(LEFT(cellBaseFilename,24)="TP_Template_Excel_module","Please select menu item  'File'&gt;'Save As...' using filename format at left, then re-open!",
  _xlfn.CONCAT(
 IF(ISERROR(INT(LEFT(cellBaseFilename,4))),"Year (filename[1-4]) NOT a number; ",IF(AND(INT(LEFT(cellBaseFilename,4))&gt;2000,INT(LEFT(cellBaseFilename,4))&lt;2100),"","Year (filename[1-4]) not between 2000 and 2100; ")),
@@ -2955,19 +2932,19 @@
 ))</f>
         <v/>
       </c>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="82"/>
+      <c r="W1" s="82"/>
+      <c r="X1" s="82"/>
+      <c r="Y1" s="82"/>
+      <c r="Z1" s="82"/>
+      <c r="AA1" s="82"/>
+      <c r="AB1" s="82"/>
+      <c r="AC1" s="82"/>
       <c r="AD1" s="29" t="s">
         <v>28</v>
       </c>
@@ -2990,12 +2967,12 @@
       <c r="A2" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="64" t="str">
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="92" t="str">
         <f ca="1">IF(LEN(cellFilenameFormatErrors)=0,
 IF(ISERROR(cellFilenameStudySectionName),
       cellFilenameStudySectionCode&amp;" is not a valid Study Section abbreviation, see [Menu Items] worksheet for the list",
@@ -3004,35 +2981,35 @@
 "Determined from the Code above (X=Study Section abbrev). See columns F and G in the 'Menu Items' tab below.")</f>
         <v>Animal DNA viruses and Retroviruses (D) proposals</v>
       </c>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="55" t="str">
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="83" t="str">
         <f ca="1">_xlfn.CONCAT(
 IF(NOT(ISERROR(AF2)),"","Study Section code ('"&amp;AE2&amp;"') is not valid; ")
 )</f>
         <v/>
       </c>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="56"/>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="56"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
+      <c r="S2" s="84"/>
+      <c r="T2" s="84"/>
+      <c r="U2" s="84"/>
+      <c r="V2" s="84"/>
+      <c r="W2" s="84"/>
+      <c r="X2" s="84"/>
+      <c r="Y2" s="84"/>
+      <c r="Z2" s="84"/>
+      <c r="AA2" s="84"/>
+      <c r="AB2" s="84"/>
+      <c r="AC2" s="84"/>
       <c r="AD2" s="30" t="s">
         <v>28</v>
       </c>
@@ -3054,53 +3031,53 @@
       <c r="AN2" s="3"/>
     </row>
     <row r="3" spans="1:41" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57"/>
-      <c r="N3" s="57"/>
-      <c r="O3" s="57"/>
-      <c r="P3" s="58" t="s">
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58"/>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58"/>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="58"/>
-      <c r="AC3" s="58"/>
-      <c r="AD3" s="58"/>
-      <c r="AE3" s="59" t="s">
+      <c r="Q3" s="86"/>
+      <c r="R3" s="86"/>
+      <c r="S3" s="86"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="86"/>
+      <c r="W3" s="86"/>
+      <c r="X3" s="86"/>
+      <c r="Y3" s="86"/>
+      <c r="Z3" s="86"/>
+      <c r="AA3" s="86"/>
+      <c r="AB3" s="86"/>
+      <c r="AC3" s="86"/>
+      <c r="AD3" s="86"/>
+      <c r="AE3" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="AF3" s="60"/>
-      <c r="AG3" s="60"/>
-      <c r="AH3" s="60"/>
-      <c r="AI3" s="60"/>
-      <c r="AJ3" s="60"/>
-      <c r="AK3" s="61"/>
-      <c r="AL3" s="51" t="s">
+      <c r="AF3" s="88"/>
+      <c r="AG3" s="88"/>
+      <c r="AH3" s="88"/>
+      <c r="AI3" s="88"/>
+      <c r="AJ3" s="88"/>
+      <c r="AK3" s="89"/>
+      <c r="AL3" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="AM3" s="52"/>
+      <c r="AM3" s="80"/>
       <c r="AN3" s="31" t="s">
         <v>23</v>
       </c>
@@ -3290,13 +3267,13 @@
         <v>125</v>
       </c>
       <c r="AE5" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="AF5" s="4" t="s">
         <v>126</v>
       </c>
       <c r="AG5" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AI5" s="4" t="s">
         <v>24</v>
@@ -3314,7 +3291,7 @@
         <v>28</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.2">
@@ -3370,16 +3347,16 @@
         <v>123</v>
       </c>
       <c r="AD6" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF6" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="AE6" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF6" s="4" t="s">
-        <v>129</v>
-      </c>
       <c r="AG6" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="AI6" s="4" t="s">
         <v>24</v>
@@ -3397,7 +3374,7 @@
         <v>28</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.2">
@@ -3453,16 +3430,16 @@
         <v>123</v>
       </c>
       <c r="AD7" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="AE7" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF7" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="AE7" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="AF7" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="AG7" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="AI7" s="4" t="s">
         <v>24</v>
@@ -3480,7 +3457,7 @@
         <v>28</v>
       </c>
       <c r="AN7" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.2">
@@ -3536,16 +3513,16 @@
         <v>123</v>
       </c>
       <c r="AD8" s="26" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="AE8" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF8" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="AF8" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="AG8" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="AI8" s="4" t="s">
         <v>24</v>
@@ -3563,7 +3540,7 @@
         <v>28</v>
       </c>
       <c r="AN8" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.2">
@@ -3589,7 +3566,7 @@
         <v>124</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="P9" s="14" t="s">
         <v>116</v>
@@ -3613,7 +3590,7 @@
         <v>124</v>
       </c>
       <c r="AB9" s="14" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AJ9" s="4" t="s">
         <v>108</v>
@@ -3625,7 +3602,7 @@
         <v>35</v>
       </c>
       <c r="AN9" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.2">
@@ -3651,7 +3628,7 @@
         <v>124</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="P10" s="14" t="s">
         <v>116</v>
@@ -3675,7 +3652,7 @@
         <v>124</v>
       </c>
       <c r="AB10" s="14" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="AJ10" s="4" t="s">
         <v>108</v>
@@ -3687,7 +3664,7 @@
         <v>35</v>
       </c>
       <c r="AN10" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:41" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3718,7 +3695,7 @@
         <v>124</v>
       </c>
       <c r="M11" s="36" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N11" s="36"/>
       <c r="O11" s="36"/>
@@ -3749,10 +3726,10 @@
         <v>124</v>
       </c>
       <c r="AB11" s="37" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="AC11" s="37" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="AD11" s="38"/>
       <c r="AE11" s="39"/>
@@ -3771,199 +3748,193 @@
         <v>32</v>
       </c>
       <c r="AN11" s="41" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:41" s="45" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66" t="s">
+      <c r="B12" s="52"/>
+      <c r="C12" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66" t="s">
+      <c r="D12" s="52"/>
+      <c r="E12" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66" t="s">
+      <c r="F12" s="52"/>
+      <c r="G12" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66" t="s">
+      <c r="H12" s="52"/>
+      <c r="I12" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="J12" s="66"/>
-      <c r="K12" s="66" t="s">
+      <c r="J12" s="52"/>
+      <c r="K12" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="L12" s="66" t="s">
+      <c r="L12" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="M12" s="66" t="s">
-        <v>149</v>
-      </c>
-      <c r="N12" s="66"/>
-      <c r="O12" s="94" t="s">
-        <v>150</v>
-      </c>
-      <c r="P12" s="67" t="s">
+      <c r="M12" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="N12" s="52"/>
+      <c r="O12" s="77" t="s">
+        <v>147</v>
+      </c>
+      <c r="P12" s="53" t="s">
         <v>116</v>
       </c>
       <c r="Q12" s="44"/>
-      <c r="R12" s="71" t="s">
+      <c r="R12" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="S12" s="71"/>
-      <c r="T12" s="71" t="s">
+      <c r="S12" s="54"/>
+      <c r="T12" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="U12" s="71"/>
-      <c r="V12" s="71" t="s">
+      <c r="U12" s="54"/>
+      <c r="V12" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="W12" s="71"/>
-      <c r="X12" s="71" t="s">
+      <c r="W12" s="54"/>
+      <c r="X12" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="Y12" s="71"/>
-      <c r="Z12" s="71" t="s">
+      <c r="Y12" s="54"/>
+      <c r="Z12" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="AA12" s="71" t="s">
+      <c r="AA12" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="AB12" s="71" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC12" s="71"/>
-      <c r="AD12" s="72" t="s">
+      <c r="AB12" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC12" s="54"/>
+      <c r="AD12" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="AE12" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="AF12" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="AG12" s="56" t="s">
         <v>151</v>
       </c>
-      <c r="AE12" s="73" t="s">
-        <v>157</v>
-      </c>
-      <c r="AF12" s="73" t="s">
+      <c r="AH12" s="56"/>
+      <c r="AI12" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ12" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK12" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL12" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="AM12" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN12" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="AG12" s="73" t="s">
-        <v>154</v>
-      </c>
-      <c r="AH12" s="73"/>
-      <c r="AI12" s="73" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ12" s="73" t="s">
-        <v>108</v>
-      </c>
-      <c r="AK12" s="73" t="s">
-        <v>63</v>
-      </c>
-      <c r="AL12" s="74" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM12" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="AN12" s="75" t="s">
-        <v>163</v>
-      </c>
-      <c r="AO12" s="76"/>
+      <c r="AO12" s="59"/>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69" t="s">
+      <c r="E13" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69" t="s">
+      <c r="G13" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="H13" s="69"/>
-      <c r="I13" s="69" t="s">
+      <c r="I13" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69" t="s">
+      <c r="K13" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="L13" s="69" t="s">
+      <c r="L13" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M13" s="69" t="s">
+      <c r="M13" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="O13" s="77" t="s">
+        <v>147</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="R13" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="S13" s="60"/>
+      <c r="T13" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="U13" s="60"/>
+      <c r="V13" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="W13" s="60"/>
+      <c r="X13" s="60" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y13" s="60"/>
+      <c r="Z13" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA13" s="60" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB13" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC13" s="60"/>
+      <c r="AD13" s="61" t="s">
         <v>149</v>
       </c>
-      <c r="N13" s="69"/>
-      <c r="O13" s="94" t="s">
-        <v>150</v>
-      </c>
-      <c r="P13" s="70" t="s">
-        <v>116</v>
-      </c>
-      <c r="R13" s="77" t="s">
-        <v>117</v>
-      </c>
-      <c r="S13" s="77"/>
-      <c r="T13" s="77" t="s">
-        <v>118</v>
-      </c>
-      <c r="U13" s="77"/>
-      <c r="V13" s="77" t="s">
-        <v>119</v>
-      </c>
-      <c r="W13" s="77"/>
-      <c r="X13" s="77" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y13" s="77"/>
-      <c r="Z13" s="77" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA13" s="77" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB13" s="77" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC13" s="77"/>
-      <c r="AD13" s="78" t="s">
+      <c r="AE13" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF13" s="56" t="s">
+        <v>158</v>
+      </c>
+      <c r="AG13" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="AE13" s="79" t="s">
-        <v>158</v>
-      </c>
-      <c r="AF13" s="73" t="s">
-        <v>161</v>
-      </c>
-      <c r="AG13" s="79" t="s">
-        <v>155</v>
-      </c>
-      <c r="AH13" s="79"/>
-      <c r="AI13" s="79" t="s">
+      <c r="AH13" s="62"/>
+      <c r="AI13" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="AJ13" s="79" t="s">
+      <c r="AJ13" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="AK13" s="79" t="s">
+      <c r="AK13" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="AL13" s="80" t="s">
+      <c r="AL13" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="AM13" s="80" t="s">
+      <c r="AM13" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="AN13" s="81"/>
-      <c r="AO13" s="82"/>
+      <c r="AN13" s="64"/>
+      <c r="AO13" s="65"/>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14" s="46" t="s">
@@ -3988,70 +3959,70 @@
         <v>122</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="O14" s="94" t="s">
-        <v>150</v>
+        <v>146</v>
+      </c>
+      <c r="O14" s="77" t="s">
+        <v>147</v>
       </c>
       <c r="P14" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="R14" s="77" t="s">
+      <c r="R14" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="S14" s="77"/>
-      <c r="T14" s="77" t="s">
+      <c r="S14" s="60"/>
+      <c r="T14" s="60" t="s">
         <v>118</v>
       </c>
-      <c r="U14" s="77"/>
-      <c r="V14" s="77" t="s">
+      <c r="U14" s="60"/>
+      <c r="V14" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="W14" s="77"/>
-      <c r="X14" s="77" t="s">
+      <c r="W14" s="60"/>
+      <c r="X14" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="Y14" s="77"/>
-      <c r="Z14" s="77" t="s">
+      <c r="Y14" s="60"/>
+      <c r="Z14" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="AA14" s="77" t="s">
+      <c r="AA14" s="60" t="s">
         <v>122</v>
       </c>
-      <c r="AB14" s="77" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC14" s="77"/>
-      <c r="AD14" s="78" t="s">
+      <c r="AB14" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC14" s="60"/>
+      <c r="AD14" s="61" t="s">
+        <v>150</v>
+      </c>
+      <c r="AE14" s="62" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF14" s="62" t="s">
+        <v>159</v>
+      </c>
+      <c r="AG14" s="62" t="s">
         <v>153</v>
       </c>
-      <c r="AE14" s="79" t="s">
-        <v>159</v>
-      </c>
-      <c r="AF14" s="79" t="s">
-        <v>162</v>
-      </c>
-      <c r="AG14" s="79" t="s">
-        <v>156</v>
-      </c>
-      <c r="AH14" s="79"/>
-      <c r="AI14" s="79" t="s">
+      <c r="AH14" s="62"/>
+      <c r="AI14" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="AJ14" s="79" t="s">
+      <c r="AJ14" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="AK14" s="79" t="s">
+      <c r="AK14" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="AL14" s="80" t="s">
+      <c r="AL14" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="AM14" s="80" t="s">
+      <c r="AM14" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="AN14" s="81"/>
-      <c r="AO14" s="82"/>
+      <c r="AN14" s="64"/>
+      <c r="AO14" s="65"/>
     </row>
     <row r="15" spans="1:41" s="50" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47"/>
@@ -4068,33 +4039,33 @@
       <c r="L15" s="48"/>
       <c r="M15" s="48"/>
       <c r="N15" s="48"/>
-      <c r="O15" s="95"/>
+      <c r="O15" s="78"/>
       <c r="P15" s="49"/>
       <c r="Q15" s="49"/>
-      <c r="R15" s="83"/>
-      <c r="S15" s="83"/>
-      <c r="T15" s="83"/>
-      <c r="U15" s="83"/>
-      <c r="V15" s="83"/>
-      <c r="W15" s="83"/>
-      <c r="X15" s="83"/>
-      <c r="Y15" s="83"/>
-      <c r="Z15" s="83"/>
-      <c r="AA15" s="83"/>
-      <c r="AB15" s="83"/>
-      <c r="AC15" s="83"/>
-      <c r="AD15" s="84"/>
-      <c r="AE15" s="85"/>
-      <c r="AF15" s="85"/>
-      <c r="AG15" s="85"/>
-      <c r="AH15" s="85"/>
-      <c r="AI15" s="85"/>
-      <c r="AJ15" s="85"/>
-      <c r="AK15" s="85"/>
-      <c r="AL15" s="86"/>
-      <c r="AM15" s="86"/>
-      <c r="AN15" s="87"/>
-      <c r="AO15" s="88"/>
+      <c r="R15" s="66"/>
+      <c r="S15" s="66"/>
+      <c r="T15" s="66"/>
+      <c r="U15" s="66"/>
+      <c r="V15" s="66"/>
+      <c r="W15" s="66"/>
+      <c r="X15" s="66"/>
+      <c r="Y15" s="66"/>
+      <c r="Z15" s="66"/>
+      <c r="AA15" s="66"/>
+      <c r="AB15" s="66"/>
+      <c r="AC15" s="66"/>
+      <c r="AD15" s="67"/>
+      <c r="AE15" s="68"/>
+      <c r="AF15" s="68"/>
+      <c r="AG15" s="68"/>
+      <c r="AH15" s="68"/>
+      <c r="AI15" s="68"/>
+      <c r="AJ15" s="68"/>
+      <c r="AK15" s="68"/>
+      <c r="AL15" s="69"/>
+      <c r="AM15" s="69"/>
+      <c r="AN15" s="70"/>
+      <c r="AO15" s="71"/>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16" s="42"/>
@@ -4114,82 +4085,82 @@
       <c r="O16" s="42"/>
       <c r="P16" s="43"/>
       <c r="Q16" s="43"/>
-      <c r="R16" s="89"/>
-      <c r="S16" s="89"/>
-      <c r="T16" s="89"/>
-      <c r="U16" s="89"/>
-      <c r="V16" s="89"/>
-      <c r="W16" s="89"/>
-      <c r="X16" s="89"/>
-      <c r="Y16" s="89"/>
-      <c r="Z16" s="89"/>
-      <c r="AA16" s="89"/>
-      <c r="AB16" s="89"/>
-      <c r="AC16" s="89"/>
-      <c r="AD16" s="90"/>
-      <c r="AE16" s="91"/>
-      <c r="AF16" s="91"/>
-      <c r="AG16" s="91"/>
-      <c r="AH16" s="91"/>
-      <c r="AI16" s="91"/>
-      <c r="AJ16" s="91"/>
-      <c r="AK16" s="91"/>
-      <c r="AL16" s="92"/>
-      <c r="AM16" s="92"/>
-      <c r="AN16" s="93"/>
-      <c r="AO16" s="82"/>
+      <c r="R16" s="72"/>
+      <c r="S16" s="72"/>
+      <c r="T16" s="72"/>
+      <c r="U16" s="72"/>
+      <c r="V16" s="72"/>
+      <c r="W16" s="72"/>
+      <c r="X16" s="72"/>
+      <c r="Y16" s="72"/>
+      <c r="Z16" s="72"/>
+      <c r="AA16" s="72"/>
+      <c r="AB16" s="72"/>
+      <c r="AC16" s="72"/>
+      <c r="AD16" s="73"/>
+      <c r="AE16" s="74"/>
+      <c r="AF16" s="74"/>
+      <c r="AG16" s="74"/>
+      <c r="AH16" s="74"/>
+      <c r="AI16" s="74"/>
+      <c r="AJ16" s="74"/>
+      <c r="AK16" s="74"/>
+      <c r="AL16" s="75"/>
+      <c r="AM16" s="75"/>
+      <c r="AN16" s="76"/>
+      <c r="AO16" s="65"/>
     </row>
     <row r="17" spans="18:41" x14ac:dyDescent="0.2">
-      <c r="R17" s="77"/>
-      <c r="S17" s="77"/>
-      <c r="T17" s="77"/>
-      <c r="U17" s="77"/>
-      <c r="V17" s="77"/>
-      <c r="W17" s="77"/>
-      <c r="X17" s="77"/>
-      <c r="Y17" s="77"/>
-      <c r="Z17" s="77"/>
-      <c r="AA17" s="77"/>
-      <c r="AB17" s="77"/>
-      <c r="AC17" s="77"/>
-      <c r="AD17" s="78"/>
-      <c r="AE17" s="79"/>
-      <c r="AF17" s="79"/>
-      <c r="AG17" s="79"/>
-      <c r="AH17" s="79"/>
-      <c r="AI17" s="79"/>
-      <c r="AJ17" s="79"/>
-      <c r="AK17" s="79"/>
-      <c r="AL17" s="80"/>
-      <c r="AM17" s="80"/>
-      <c r="AN17" s="81"/>
-      <c r="AO17" s="82"/>
+      <c r="R17" s="60"/>
+      <c r="S17" s="60"/>
+      <c r="T17" s="60"/>
+      <c r="U17" s="60"/>
+      <c r="V17" s="60"/>
+      <c r="W17" s="60"/>
+      <c r="X17" s="60"/>
+      <c r="Y17" s="60"/>
+      <c r="Z17" s="60"/>
+      <c r="AA17" s="60"/>
+      <c r="AB17" s="60"/>
+      <c r="AC17" s="60"/>
+      <c r="AD17" s="61"/>
+      <c r="AE17" s="62"/>
+      <c r="AF17" s="62"/>
+      <c r="AG17" s="62"/>
+      <c r="AH17" s="62"/>
+      <c r="AI17" s="62"/>
+      <c r="AJ17" s="62"/>
+      <c r="AK17" s="62"/>
+      <c r="AL17" s="63"/>
+      <c r="AM17" s="63"/>
+      <c r="AN17" s="64"/>
+      <c r="AO17" s="65"/>
     </row>
     <row r="18" spans="18:41" x14ac:dyDescent="0.2">
-      <c r="R18" s="77"/>
-      <c r="S18" s="77"/>
-      <c r="T18" s="77"/>
-      <c r="U18" s="77"/>
-      <c r="V18" s="77"/>
-      <c r="W18" s="77"/>
-      <c r="X18" s="77"/>
-      <c r="Y18" s="77"/>
-      <c r="Z18" s="77"/>
-      <c r="AA18" s="77"/>
-      <c r="AB18" s="77"/>
-      <c r="AC18" s="77"/>
-      <c r="AD18" s="78"/>
-      <c r="AE18" s="79"/>
-      <c r="AF18" s="79"/>
-      <c r="AG18" s="79"/>
-      <c r="AH18" s="79"/>
-      <c r="AI18" s="79"/>
-      <c r="AJ18" s="79"/>
-      <c r="AK18" s="79"/>
-      <c r="AL18" s="80"/>
-      <c r="AM18" s="80"/>
-      <c r="AN18" s="81"/>
-      <c r="AO18" s="82"/>
+      <c r="R18" s="60"/>
+      <c r="S18" s="60"/>
+      <c r="T18" s="60"/>
+      <c r="U18" s="60"/>
+      <c r="V18" s="60"/>
+      <c r="W18" s="60"/>
+      <c r="X18" s="60"/>
+      <c r="Y18" s="60"/>
+      <c r="Z18" s="60"/>
+      <c r="AA18" s="60"/>
+      <c r="AB18" s="60"/>
+      <c r="AC18" s="60"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="62"/>
+      <c r="AF18" s="62"/>
+      <c r="AG18" s="62"/>
+      <c r="AH18" s="62"/>
+      <c r="AI18" s="62"/>
+      <c r="AJ18" s="62"/>
+      <c r="AK18" s="62"/>
+      <c r="AL18" s="63"/>
+      <c r="AM18" s="63"/>
+      <c r="AN18" s="64"/>
+      <c r="AO18" s="65"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" insertRows="0" insertHyperlinks="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -4206,32 +4177,32 @@
     <mergeCell ref="E2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:AD1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>ROW(A1)&gt;5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048574 Q3:AC1048574">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>AND(NOT(ISBLANK(P1)),COUNTA(Q1:$AD1)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:AC1048576">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text=" ">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text=" ">
       <formula>NOT(ISERROR(SEARCH(" ",P4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1048575:AC1048576">
-    <cfRule type="expression" dxfId="7" priority="22">
+    <cfRule type="expression" dxfId="2" priority="22">
       <formula>AND(NOT(ISBLANK(P1048575)),COUNTA(Q1048575:$AD1048576)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD1:AD1048576">
-    <cfRule type="expression" dxfId="6" priority="17">
+    <cfRule type="expression" dxfId="1" priority="17">
       <formula>NOT(OR(OR(AD1="",AD1="Species"),_xlfn.CONCAT(AB1," ")=LEFT(AD1,LEN(AB1)+1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM4:AM1048576">
-    <cfRule type="expression" dxfId="5" priority="19">
+    <cfRule type="expression" dxfId="0" priority="19">
       <formula>NOT(AM4=proposedRank)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>